<commit_message>
explain about github copilot
</commit_message>
<xml_diff>
--- a/img/img.xlsx
+++ b/img/img.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/72b25cd276dfe419/デスクトップ/deploy/Netsugen-GitHub/img/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="13_ncr:1_{B9C16733-1462-4A32-B2CA-9CF495B3ABA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CE6412E-B46D-46CF-AD65-E9235EC74466}"/>
+  <xr:revisionPtr revIDLastSave="148" documentId="13_ncr:1_{B9C16733-1462-4A32-B2CA-9CF495B3ABA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4155474-7F9A-4DE9-9498-BE63C6FEF34B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="codespace" sheetId="3" r:id="rId1"/>
-    <sheet name="secret" sheetId="2" r:id="rId2"/>
-    <sheet name="blank" sheetId="1" r:id="rId3"/>
+    <sheet name="copilot" sheetId="4" r:id="rId1"/>
+    <sheet name="codespace" sheetId="3" r:id="rId2"/>
+    <sheet name="secret" sheetId="2" r:id="rId3"/>
+    <sheet name="blank" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,10 +25,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -97,25 +94,164 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>166789</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>29308</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>63</xdr:col>
+      <xdr:colOff>58617</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>87821</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="図 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0BD2C94-DB17-CA40-0A63-097CA54A2648}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="166789" y="227135"/>
+          <a:ext cx="12354924" cy="5202013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>189638</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>63</xdr:col>
+      <xdr:colOff>21981</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>159024</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="図 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A222F9F0-E9B8-0505-7F7E-6E1D324D80A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="189638" y="5634403"/>
+          <a:ext cx="12295439" cy="4415967"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>48764</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>181936</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>63</xdr:col>
+      <xdr:colOff>86591</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>26333</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="図 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA1DB011-649C-B04D-9AC8-B82E7ED6728F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="256582" y="10780663"/>
+          <a:ext cx="12922554" cy="5871125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>102178</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>65232</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>111702</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>106507</xdr:rowOff>
+      <xdr:col>80</xdr:col>
+      <xdr:colOff>31839</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>22</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>84</xdr:col>
+      <xdr:colOff>41363</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>41298</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="2" name="直線矢印コネクタ 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9E0FC39-095D-46F4-966E-7DE941B777F1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E09F297-5CB6-4E98-BBFC-C817A6900779}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -123,8 +259,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5502853" y="3265632"/>
-          <a:ext cx="809624" cy="1241425"/>
+          <a:off x="16033839" y="11201422"/>
+          <a:ext cx="809624" cy="1241426"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -155,23 +291,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>49068</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>163366</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>68117</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>39542</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>167638</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>145959</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>85397</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>19707</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="正方形/長方形 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B49390D8-FB95-422A-9C7A-CB2EA8C6B6BE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D9BF7FD-6D1D-46C4-A475-0686BAF09ED2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -179,8 +315,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4849668" y="1963591"/>
-          <a:ext cx="2819399" cy="1276351"/>
+          <a:off x="2335397" y="15517338"/>
+          <a:ext cx="706034" cy="267886"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -221,23 +357,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>123248</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>80531</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>1155</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>13855</xdr:rowOff>
+      <xdr:col>67</xdr:col>
+      <xdr:colOff>18473</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>137681</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>83</xdr:col>
+      <xdr:colOff>96405</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>71005</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="4" name="吹き出し: 四角形 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D34B88D2-425F-4BC6-A87E-92DE6B6A0389}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A68F5D95-565A-458C-86AB-72F3E15A3C98}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -245,7 +381,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4523798" y="1080656"/>
+          <a:off x="13420148" y="10538981"/>
           <a:ext cx="3278332" cy="533399"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
@@ -308,10 +444,292 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>155814</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>35600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>6568</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>111673</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="正方形/長方形 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED3080D0-89CB-42A8-8A0F-4DF60CBE1549}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4294262" y="13633359"/>
+          <a:ext cx="6156961" cy="1258486"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>102178</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>65232</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>111702</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>106507</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="直線矢印コネクタ 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9E0FC39-095D-46F4-966E-7DE941B777F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5502853" y="3265632"/>
+          <a:ext cx="809624" cy="1241425"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>49068</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>163366</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>68117</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>39542</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="正方形/長方形 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B49390D8-FB95-422A-9C7A-CB2EA8C6B6BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4849668" y="1963591"/>
+          <a:ext cx="2819399" cy="1276351"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>123248</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>80531</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>1155</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>13855</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="吹き出し: 四角形 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D34B88D2-425F-4BC6-A87E-92DE6B6A0389}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4523798" y="1080656"/>
+          <a:ext cx="3278332" cy="533399"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -55152"/>
+            <a:gd name="adj2" fmla="val 13397"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Gmail</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>のアドレス、パスワードを入力</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1572,7 +1990,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2050,10 +2468,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E992BAF8-9F03-4837-9E2B-FA492B1B0B28}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8737B700-C5D4-4F86-A921-1B9BD3A7E5F0}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="BZ73" sqref="BZ73"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="15.75"/>
   <cols>
@@ -2067,11 +2487,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E992BAF8-9F03-4837-9E2B-FA492B1B0B28}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="16384" width="2.625" style="1"/>
+  </cols>
+  <sheetData/>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE33003-F266-4BB6-8726-AD6596FC1B75}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="B217" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N243" sqref="N243"/>
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="BX24" sqref="BX24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="15.75"/>
@@ -2086,7 +2525,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>